<commit_message>
Update properties and variables related to votes in multiple files
</commit_message>
<xml_diff>
--- a/DatalexionBackend/DatalexionBackend.UI/wwwroot/Circuitos_upload.xlsx
+++ b/DatalexionBackend/DatalexionBackend.UI/wwwroot/Circuitos_upload.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DatalexionSolution\DatalexionBackend\DatalexionBackend.UI\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\DatalexionSolution\DatalexionBackend\DatalexionBackend.UI\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20491" windowHeight="9202"/>
   </bookViews>
   <sheets>
     <sheet name="Plan Circuital - Versión 3" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <t>DEPARTAMENTO</t>
   </si>
   <si>
-    <t>Santa Lucía</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -427,23 +427,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -694,10 +678,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15.2" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.25" customWidth="1"/>
     <col min="3" max="3" width="12.125" customWidth="1"/>
@@ -710,7 +694,7 @@
     <col min="10" max="27" width="96.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>30</v>
       </c>
@@ -742,7 +726,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2056</v>
       </c>
@@ -774,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2066</v>
       </c>
@@ -806,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2073</v>
       </c>
@@ -838,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2079</v>
       </c>
@@ -870,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>2083</v>
       </c>
@@ -902,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2091</v>
       </c>
@@ -934,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2098</v>
       </c>
@@ -966,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2105</v>
       </c>
@@ -998,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2114</v>
       </c>
@@ -1030,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2136</v>
       </c>
@@ -1062,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2143</v>
       </c>
@@ -1094,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>2159</v>
       </c>
@@ -1126,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2167</v>
       </c>
@@ -1158,12 +1142,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2168</v>
       </c>
       <c r="B15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>42</v>
@@ -1190,12 +1174,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2169</v>
       </c>
       <c r="B16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
@@ -1222,12 +1206,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2170</v>
       </c>
       <c r="B17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
@@ -1254,12 +1238,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2171</v>
       </c>
       <c r="B18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
@@ -1286,12 +1270,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2172</v>
       </c>
       <c r="B19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>42</v>
@@ -1318,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1347,7 +1331,7 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1376,7 +1360,7 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1405,7 +1389,7 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1434,7 +1418,7 @@
       <c r="Z23" s="8"/>
       <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1463,7 +1447,7 @@
       <c r="Z24" s="8"/>
       <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1492,7 +1476,7 @@
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1521,7 +1505,7 @@
       <c r="Z26" s="8"/>
       <c r="AA26" s="8"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1550,7 +1534,7 @@
       <c r="Z27" s="8"/>
       <c r="AA27" s="8"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1579,7 +1563,7 @@
       <c r="Z28" s="8"/>
       <c r="AA28" s="8"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1608,7 +1592,7 @@
       <c r="Z29" s="8"/>
       <c r="AA29" s="8"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1637,7 +1621,7 @@
       <c r="Z30" s="8"/>
       <c r="AA30" s="8"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1666,7 +1650,7 @@
       <c r="Z31" s="8"/>
       <c r="AA31" s="8"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1695,7 +1679,7 @@
       <c r="Z32" s="8"/>
       <c r="AA32" s="8"/>
     </row>
-    <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1724,7 +1708,7 @@
       <c r="Z33" s="8"/>
       <c r="AA33" s="8"/>
     </row>
-    <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1753,7 +1737,7 @@
       <c r="Z34" s="8"/>
       <c r="AA34" s="8"/>
     </row>
-    <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1782,7 +1766,7 @@
       <c r="Z35" s="8"/>
       <c r="AA35" s="8"/>
     </row>
-    <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1811,7 +1795,7 @@
       <c r="Z36" s="8"/>
       <c r="AA36" s="8"/>
     </row>
-    <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1840,7 +1824,7 @@
       <c r="Z37" s="8"/>
       <c r="AA37" s="8"/>
     </row>
-    <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1869,7 +1853,7 @@
       <c r="Z38" s="8"/>
       <c r="AA38" s="8"/>
     </row>
-    <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1898,7 +1882,7 @@
       <c r="Z39" s="8"/>
       <c r="AA39" s="8"/>
     </row>
-    <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1927,7 +1911,7 @@
       <c r="Z40" s="8"/>
       <c r="AA40" s="8"/>
     </row>
-    <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1956,7 +1940,7 @@
       <c r="Z41" s="8"/>
       <c r="AA41" s="8"/>
     </row>
-    <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1985,7 +1969,7 @@
       <c r="Z42" s="8"/>
       <c r="AA42" s="8"/>
     </row>
-    <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2014,7 +1998,7 @@
       <c r="Z43" s="8"/>
       <c r="AA43" s="8"/>
     </row>
-    <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2043,7 +2027,7 @@
       <c r="Z44" s="8"/>
       <c r="AA44" s="8"/>
     </row>
-    <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -2072,7 +2056,7 @@
       <c r="Z45" s="8"/>
       <c r="AA45" s="8"/>
     </row>
-    <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2101,7 +2085,7 @@
       <c r="Z46" s="8"/>
       <c r="AA46" s="8"/>
     </row>
-    <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2130,7 +2114,7 @@
       <c r="Z47" s="8"/>
       <c r="AA47" s="8"/>
     </row>
-    <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -2159,7 +2143,7 @@
       <c r="Z48" s="8"/>
       <c r="AA48" s="8"/>
     </row>
-    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2188,7 +2172,7 @@
       <c r="Z49" s="8"/>
       <c r="AA49" s="8"/>
     </row>
-    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2217,7 +2201,7 @@
       <c r="Z50" s="8"/>
       <c r="AA50" s="8"/>
     </row>
-    <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -2246,7 +2230,7 @@
       <c r="Z51" s="8"/>
       <c r="AA51" s="8"/>
     </row>
-    <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -2275,7 +2259,7 @@
       <c r="Z52" s="8"/>
       <c r="AA52" s="8"/>
     </row>
-    <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2304,7 +2288,7 @@
       <c r="Z53" s="8"/>
       <c r="AA53" s="8"/>
     </row>
-    <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -2333,7 +2317,7 @@
       <c r="Z54" s="8"/>
       <c r="AA54" s="8"/>
     </row>
-    <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -2362,7 +2346,7 @@
       <c r="Z55" s="8"/>
       <c r="AA55" s="8"/>
     </row>
-    <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -2391,7 +2375,7 @@
       <c r="Z56" s="8"/>
       <c r="AA56" s="8"/>
     </row>
-    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -2420,7 +2404,7 @@
       <c r="Z57" s="8"/>
       <c r="AA57" s="8"/>
     </row>
-    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -2449,7 +2433,7 @@
       <c r="Z58" s="8"/>
       <c r="AA58" s="8"/>
     </row>
-    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -2478,7 +2462,7 @@
       <c r="Z59" s="8"/>
       <c r="AA59" s="8"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -2507,7 +2491,7 @@
       <c r="Z60" s="8"/>
       <c r="AA60" s="8"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -2536,7 +2520,7 @@
       <c r="Z61" s="8"/>
       <c r="AA61" s="8"/>
     </row>
-    <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -2565,7 +2549,7 @@
       <c r="Z62" s="8"/>
       <c r="AA62" s="8"/>
     </row>
-    <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -2594,7 +2578,7 @@
       <c r="Z63" s="8"/>
       <c r="AA63" s="8"/>
     </row>
-    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -2623,7 +2607,7 @@
       <c r="Z64" s="8"/>
       <c r="AA64" s="8"/>
     </row>
-    <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -2652,7 +2636,7 @@
       <c r="Z65" s="8"/>
       <c r="AA65" s="8"/>
     </row>
-    <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -2681,7 +2665,7 @@
       <c r="Z66" s="8"/>
       <c r="AA66" s="8"/>
     </row>
-    <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -2710,7 +2694,7 @@
       <c r="Z67" s="8"/>
       <c r="AA67" s="8"/>
     </row>
-    <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -2739,7 +2723,7 @@
       <c r="Z68" s="8"/>
       <c r="AA68" s="8"/>
     </row>
-    <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2768,7 +2752,7 @@
       <c r="Z69" s="8"/>
       <c r="AA69" s="8"/>
     </row>
-    <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2797,7 +2781,7 @@
       <c r="Z70" s="8"/>
       <c r="AA70" s="8"/>
     </row>
-    <row r="71" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -2826,7 +2810,7 @@
       <c r="Z71" s="8"/>
       <c r="AA71" s="8"/>
     </row>
-    <row r="72" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -2855,7 +2839,7 @@
       <c r="Z72" s="8"/>
       <c r="AA72" s="8"/>
     </row>
-    <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2884,7 +2868,7 @@
       <c r="Z73" s="8"/>
       <c r="AA73" s="8"/>
     </row>
-    <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2913,7 +2897,7 @@
       <c r="Z74" s="8"/>
       <c r="AA74" s="8"/>
     </row>
-    <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2942,7 +2926,7 @@
       <c r="Z75" s="8"/>
       <c r="AA75" s="8"/>
     </row>
-    <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2971,7 +2955,7 @@
       <c r="Z76" s="8"/>
       <c r="AA76" s="8"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -3000,7 +2984,7 @@
       <c r="Z77" s="8"/>
       <c r="AA77" s="8"/>
     </row>
-    <row r="78" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -3029,7 +3013,7 @@
       <c r="Z78" s="8"/>
       <c r="AA78" s="8"/>
     </row>
-    <row r="79" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -3058,7 +3042,7 @@
       <c r="Z79" s="8"/>
       <c r="AA79" s="8"/>
     </row>
-    <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -3087,7 +3071,7 @@
       <c r="Z80" s="8"/>
       <c r="AA80" s="8"/>
     </row>
-    <row r="81" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -3116,7 +3100,7 @@
       <c r="Z81" s="8"/>
       <c r="AA81" s="8"/>
     </row>
-    <row r="82" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -3145,7 +3129,7 @@
       <c r="Z82" s="8"/>
       <c r="AA82" s="8"/>
     </row>
-    <row r="83" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -3174,7 +3158,7 @@
       <c r="Z83" s="8"/>
       <c r="AA83" s="8"/>
     </row>
-    <row r="84" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -3203,7 +3187,7 @@
       <c r="Z84" s="8"/>
       <c r="AA84" s="8"/>
     </row>
-    <row r="85" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -3232,7 +3216,7 @@
       <c r="Z85" s="8"/>
       <c r="AA85" s="8"/>
     </row>
-    <row r="86" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -3261,7 +3245,7 @@
       <c r="Z86" s="8"/>
       <c r="AA86" s="8"/>
     </row>
-    <row r="87" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -3290,7 +3274,7 @@
       <c r="Z87" s="8"/>
       <c r="AA87" s="8"/>
     </row>
-    <row r="88" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -3319,7 +3303,7 @@
       <c r="Z88" s="8"/>
       <c r="AA88" s="8"/>
     </row>
-    <row r="89" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -3348,7 +3332,7 @@
       <c r="Z89" s="8"/>
       <c r="AA89" s="8"/>
     </row>
-    <row r="90" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3377,7 +3361,7 @@
       <c r="Z90" s="8"/>
       <c r="AA90" s="8"/>
     </row>
-    <row r="91" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -3406,7 +3390,7 @@
       <c r="Z91" s="8"/>
       <c r="AA91" s="8"/>
     </row>
-    <row r="92" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3435,7 +3419,7 @@
       <c r="Z92" s="8"/>
       <c r="AA92" s="8"/>
     </row>
-    <row r="93" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3464,7 +3448,7 @@
       <c r="Z93" s="8"/>
       <c r="AA93" s="8"/>
     </row>
-    <row r="94" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3493,7 +3477,7 @@
       <c r="Z94" s="8"/>
       <c r="AA94" s="8"/>
     </row>
-    <row r="95" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3522,7 +3506,7 @@
       <c r="Z95" s="8"/>
       <c r="AA95" s="8"/>
     </row>
-    <row r="96" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3551,7 +3535,7 @@
       <c r="Z96" s="8"/>
       <c r="AA96" s="8"/>
     </row>
-    <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -3580,7 +3564,7 @@
       <c r="Z97" s="8"/>
       <c r="AA97" s="8"/>
     </row>
-    <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -3609,7 +3593,7 @@
       <c r="Z98" s="8"/>
       <c r="AA98" s="8"/>
     </row>
-    <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -3638,7 +3622,7 @@
       <c r="Z99" s="8"/>
       <c r="AA99" s="8"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -3667,7 +3651,7 @@
       <c r="Z100" s="8"/>
       <c r="AA100" s="8"/>
     </row>
-    <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -3696,7 +3680,7 @@
       <c r="Z101" s="8"/>
       <c r="AA101" s="8"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3725,7 +3709,7 @@
       <c r="Z102" s="8"/>
       <c r="AA102" s="8"/>
     </row>
-    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3754,7 +3738,7 @@
       <c r="Z103" s="8"/>
       <c r="AA103" s="8"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3783,7 +3767,7 @@
       <c r="Z104" s="8"/>
       <c r="AA104" s="8"/>
     </row>
-    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3812,7 +3796,7 @@
       <c r="Z105" s="8"/>
       <c r="AA105" s="8"/>
     </row>
-    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3841,7 +3825,7 @@
       <c r="Z106" s="8"/>
       <c r="AA106" s="8"/>
     </row>
-    <row r="107" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3870,7 +3854,7 @@
       <c r="Z107" s="8"/>
       <c r="AA107" s="8"/>
     </row>
-    <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3899,7 +3883,7 @@
       <c r="Z108" s="8"/>
       <c r="AA108" s="8"/>
     </row>
-    <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -3928,7 +3912,7 @@
       <c r="Z109" s="8"/>
       <c r="AA109" s="8"/>
     </row>
-    <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -3957,7 +3941,7 @@
       <c r="Z110" s="8"/>
       <c r="AA110" s="8"/>
     </row>
-    <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -3986,7 +3970,7 @@
       <c r="Z111" s="8"/>
       <c r="AA111" s="8"/>
     </row>
-    <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -4015,7 +3999,7 @@
       <c r="Z112" s="8"/>
       <c r="AA112" s="8"/>
     </row>
-    <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -4044,7 +4028,7 @@
       <c r="Z113" s="8"/>
       <c r="AA113" s="8"/>
     </row>
-    <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -4073,7 +4057,7 @@
       <c r="Z114" s="8"/>
       <c r="AA114" s="8"/>
     </row>
-    <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -4102,7 +4086,7 @@
       <c r="Z115" s="8"/>
       <c r="AA115" s="8"/>
     </row>
-    <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -4131,7 +4115,7 @@
       <c r="Z116" s="8"/>
       <c r="AA116" s="8"/>
     </row>
-    <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -4160,7 +4144,7 @@
       <c r="Z117" s="8"/>
       <c r="AA117" s="8"/>
     </row>
-    <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -4189,7 +4173,7 @@
       <c r="Z118" s="8"/>
       <c r="AA118" s="8"/>
     </row>
-    <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -4218,7 +4202,7 @@
       <c r="Z119" s="8"/>
       <c r="AA119" s="8"/>
     </row>
-    <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -4247,7 +4231,7 @@
       <c r="Z120" s="8"/>
       <c r="AA120" s="8"/>
     </row>
-    <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -4276,7 +4260,7 @@
       <c r="Z121" s="8"/>
       <c r="AA121" s="8"/>
     </row>
-    <row r="122" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -4305,7 +4289,7 @@
       <c r="Z122" s="8"/>
       <c r="AA122" s="8"/>
     </row>
-    <row r="123" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -4334,7 +4318,7 @@
       <c r="Z123" s="8"/>
       <c r="AA123" s="8"/>
     </row>
-    <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -4363,7 +4347,7 @@
       <c r="Z124" s="8"/>
       <c r="AA124" s="8"/>
     </row>
-    <row r="125" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -4392,7 +4376,7 @@
       <c r="Z125" s="8"/>
       <c r="AA125" s="8"/>
     </row>
-    <row r="126" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
@@ -4421,7 +4405,7 @@
       <c r="Z126" s="8"/>
       <c r="AA126" s="8"/>
     </row>
-    <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
@@ -4450,7 +4434,7 @@
       <c r="Z127" s="8"/>
       <c r="AA127" s="8"/>
     </row>
-    <row r="128" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -4479,7 +4463,7 @@
       <c r="Z128" s="8"/>
       <c r="AA128" s="8"/>
     </row>
-    <row r="129" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -4508,7 +4492,7 @@
       <c r="Z129" s="8"/>
       <c r="AA129" s="8"/>
     </row>
-    <row r="130" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -4537,7 +4521,7 @@
       <c r="Z130" s="8"/>
       <c r="AA130" s="8"/>
     </row>
-    <row r="131" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -4566,7 +4550,7 @@
       <c r="Z131" s="8"/>
       <c r="AA131" s="8"/>
     </row>
-    <row r="132" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -4595,7 +4579,7 @@
       <c r="Z132" s="8"/>
       <c r="AA132" s="8"/>
     </row>
-    <row r="133" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -4624,7 +4608,7 @@
       <c r="Z133" s="8"/>
       <c r="AA133" s="8"/>
     </row>
-    <row r="134" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -4653,7 +4637,7 @@
       <c r="Z134" s="8"/>
       <c r="AA134" s="8"/>
     </row>
-    <row r="135" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -4682,7 +4666,7 @@
       <c r="Z135" s="8"/>
       <c r="AA135" s="8"/>
     </row>
-    <row r="136" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -4711,7 +4695,7 @@
       <c r="Z136" s="8"/>
       <c r="AA136" s="8"/>
     </row>
-    <row r="137" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -4740,7 +4724,7 @@
       <c r="Z137" s="8"/>
       <c r="AA137" s="8"/>
     </row>
-    <row r="138" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -4769,7 +4753,7 @@
       <c r="Z138" s="8"/>
       <c r="AA138" s="8"/>
     </row>
-    <row r="139" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -4798,7 +4782,7 @@
       <c r="Z139" s="8"/>
       <c r="AA139" s="8"/>
     </row>
-    <row r="140" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -4827,7 +4811,7 @@
       <c r="Z140" s="8"/>
       <c r="AA140" s="8"/>
     </row>
-    <row r="141" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -4856,7 +4840,7 @@
       <c r="Z141" s="8"/>
       <c r="AA141" s="8"/>
     </row>
-    <row r="142" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -4885,7 +4869,7 @@
       <c r="Z142" s="8"/>
       <c r="AA142" s="8"/>
     </row>
-    <row r="143" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -4914,7 +4898,7 @@
       <c r="Z143" s="8"/>
       <c r="AA143" s="8"/>
     </row>
-    <row r="144" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -4943,7 +4927,7 @@
       <c r="Z144" s="8"/>
       <c r="AA144" s="8"/>
     </row>
-    <row r="145" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -4972,7 +4956,7 @@
       <c r="Z145" s="8"/>
       <c r="AA145" s="8"/>
     </row>
-    <row r="146" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -5001,7 +4985,7 @@
       <c r="Z146" s="8"/>
       <c r="AA146" s="8"/>
     </row>
-    <row r="147" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -5030,7 +5014,7 @@
       <c r="Z147" s="8"/>
       <c r="AA147" s="8"/>
     </row>
-    <row r="148" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
@@ -5059,7 +5043,7 @@
       <c r="Z148" s="8"/>
       <c r="AA148" s="8"/>
     </row>
-    <row r="149" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -5088,7 +5072,7 @@
       <c r="Z149" s="8"/>
       <c r="AA149" s="8"/>
     </row>
-    <row r="150" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -5117,7 +5101,7 @@
       <c r="Z150" s="8"/>
       <c r="AA150" s="8"/>
     </row>
-    <row r="151" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -5146,7 +5130,7 @@
       <c r="Z151" s="8"/>
       <c r="AA151" s="8"/>
     </row>
-    <row r="152" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -5175,7 +5159,7 @@
       <c r="Z152" s="8"/>
       <c r="AA152" s="8"/>
     </row>
-    <row r="153" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -5204,7 +5188,7 @@
       <c r="Z153" s="8"/>
       <c r="AA153" s="8"/>
     </row>
-    <row r="154" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -5233,7 +5217,7 @@
       <c r="Z154" s="8"/>
       <c r="AA154" s="8"/>
     </row>
-    <row r="155" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -5262,7 +5246,7 @@
       <c r="Z155" s="8"/>
       <c r="AA155" s="8"/>
     </row>
-    <row r="156" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -5291,7 +5275,7 @@
       <c r="Z156" s="8"/>
       <c r="AA156" s="8"/>
     </row>
-    <row r="157" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -5320,7 +5304,7 @@
       <c r="Z157" s="8"/>
       <c r="AA157" s="8"/>
     </row>
-    <row r="158" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
@@ -5349,7 +5333,7 @@
       <c r="Z158" s="8"/>
       <c r="AA158" s="8"/>
     </row>
-    <row r="159" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
@@ -5378,7 +5362,7 @@
       <c r="Z159" s="8"/>
       <c r="AA159" s="8"/>
     </row>
-    <row r="160" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -5407,7 +5391,7 @@
       <c r="Z160" s="8"/>
       <c r="AA160" s="8"/>
     </row>
-    <row r="161" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -5436,7 +5420,7 @@
       <c r="Z161" s="8"/>
       <c r="AA161" s="8"/>
     </row>
-    <row r="162" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -5465,7 +5449,7 @@
       <c r="Z162" s="8"/>
       <c r="AA162" s="8"/>
     </row>
-    <row r="163" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -5494,7 +5478,7 @@
       <c r="Z163" s="8"/>
       <c r="AA163" s="8"/>
     </row>
-    <row r="164" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -5523,7 +5507,7 @@
       <c r="Z164" s="8"/>
       <c r="AA164" s="8"/>
     </row>
-    <row r="165" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -5552,7 +5536,7 @@
       <c r="Z165" s="8"/>
       <c r="AA165" s="8"/>
     </row>
-    <row r="166" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -5581,7 +5565,7 @@
       <c r="Z166" s="8"/>
       <c r="AA166" s="8"/>
     </row>
-    <row r="167" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -5610,7 +5594,7 @@
       <c r="Z167" s="8"/>
       <c r="AA167" s="8"/>
     </row>
-    <row r="168" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -5639,7 +5623,7 @@
       <c r="Z168" s="8"/>
       <c r="AA168" s="8"/>
     </row>
-    <row r="169" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -5668,7 +5652,7 @@
       <c r="Z169" s="8"/>
       <c r="AA169" s="8"/>
     </row>
-    <row r="170" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -5697,7 +5681,7 @@
       <c r="Z170" s="8"/>
       <c r="AA170" s="8"/>
     </row>
-    <row r="171" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -5726,7 +5710,7 @@
       <c r="Z171" s="8"/>
       <c r="AA171" s="8"/>
     </row>
-    <row r="172" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -5755,7 +5739,7 @@
       <c r="Z172" s="8"/>
       <c r="AA172" s="8"/>
     </row>
-    <row r="173" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -5784,7 +5768,7 @@
       <c r="Z173" s="8"/>
       <c r="AA173" s="8"/>
     </row>
-    <row r="174" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -5813,7 +5797,7 @@
       <c r="Z174" s="8"/>
       <c r="AA174" s="8"/>
     </row>
-    <row r="175" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -5842,7 +5826,7 @@
       <c r="Z175" s="8"/>
       <c r="AA175" s="8"/>
     </row>
-    <row r="176" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -5871,7 +5855,7 @@
       <c r="Z176" s="8"/>
       <c r="AA176" s="8"/>
     </row>
-    <row r="177" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -5900,7 +5884,7 @@
       <c r="Z177" s="8"/>
       <c r="AA177" s="8"/>
     </row>
-    <row r="178" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -5929,7 +5913,7 @@
       <c r="Z178" s="8"/>
       <c r="AA178" s="8"/>
     </row>
-    <row r="179" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -5958,7 +5942,7 @@
       <c r="Z179" s="8"/>
       <c r="AA179" s="8"/>
     </row>
-    <row r="180" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -5987,7 +5971,7 @@
       <c r="Z180" s="8"/>
       <c r="AA180" s="8"/>
     </row>
-    <row r="181" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -6016,7 +6000,7 @@
       <c r="Z181" s="8"/>
       <c r="AA181" s="8"/>
     </row>
-    <row r="182" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -6045,7 +6029,7 @@
       <c r="Z182" s="8"/>
       <c r="AA182" s="8"/>
     </row>
-    <row r="183" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -6074,7 +6058,7 @@
       <c r="Z183" s="8"/>
       <c r="AA183" s="8"/>
     </row>
-    <row r="184" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -6103,7 +6087,7 @@
       <c r="Z184" s="8"/>
       <c r="AA184" s="8"/>
     </row>
-    <row r="185" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -6132,7 +6116,7 @@
       <c r="Z185" s="8"/>
       <c r="AA185" s="8"/>
     </row>
-    <row r="186" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -6161,7 +6145,7 @@
       <c r="Z186" s="8"/>
       <c r="AA186" s="8"/>
     </row>
-    <row r="187" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -6190,7 +6174,7 @@
       <c r="Z187" s="8"/>
       <c r="AA187" s="8"/>
     </row>
-    <row r="188" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -6219,7 +6203,7 @@
       <c r="Z188" s="8"/>
       <c r="AA188" s="8"/>
     </row>
-    <row r="189" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -6248,7 +6232,7 @@
       <c r="Z189" s="8"/>
       <c r="AA189" s="8"/>
     </row>
-    <row r="190" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -6277,7 +6261,7 @@
       <c r="Z190" s="8"/>
       <c r="AA190" s="8"/>
     </row>
-    <row r="191" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -6306,7 +6290,7 @@
       <c r="Z191" s="8"/>
       <c r="AA191" s="8"/>
     </row>
-    <row r="192" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -6335,7 +6319,7 @@
       <c r="Z192" s="8"/>
       <c r="AA192" s="8"/>
     </row>
-    <row r="193" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -6364,7 +6348,7 @@
       <c r="Z193" s="8"/>
       <c r="AA193" s="8"/>
     </row>
-    <row r="194" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -6393,7 +6377,7 @@
       <c r="Z194" s="8"/>
       <c r="AA194" s="8"/>
     </row>
-    <row r="195" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -6422,7 +6406,7 @@
       <c r="Z195" s="8"/>
       <c r="AA195" s="8"/>
     </row>
-    <row r="196" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -6451,7 +6435,7 @@
       <c r="Z196" s="8"/>
       <c r="AA196" s="8"/>
     </row>
-    <row r="197" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -6480,7 +6464,7 @@
       <c r="Z197" s="8"/>
       <c r="AA197" s="8"/>
     </row>
-    <row r="198" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -6509,7 +6493,7 @@
       <c r="Z198" s="8"/>
       <c r="AA198" s="8"/>
     </row>
-    <row r="199" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -6538,7 +6522,7 @@
       <c r="Z199" s="8"/>
       <c r="AA199" s="8"/>
     </row>
-    <row r="200" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="7"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
@@ -6567,7 +6551,7 @@
       <c r="Z200" s="8"/>
       <c r="AA200" s="8"/>
     </row>
-    <row r="201" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="7"/>
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
@@ -6596,7 +6580,7 @@
       <c r="Z201" s="8"/>
       <c r="AA201" s="8"/>
     </row>
-    <row r="202" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="7"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
@@ -6625,7 +6609,7 @@
       <c r="Z202" s="8"/>
       <c r="AA202" s="8"/>
     </row>
-    <row r="203" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="7"/>
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
@@ -6654,7 +6638,7 @@
       <c r="Z203" s="8"/>
       <c r="AA203" s="8"/>
     </row>
-    <row r="204" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="7"/>
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
@@ -6683,7 +6667,7 @@
       <c r="Z204" s="8"/>
       <c r="AA204" s="8"/>
     </row>
-    <row r="205" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="7"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
@@ -6712,7 +6696,7 @@
       <c r="Z205" s="8"/>
       <c r="AA205" s="8"/>
     </row>
-    <row r="206" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:27" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="7"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>

</xml_diff>